<commit_message>
Spieler kann Startort definieren und wird in der Datenbank gespeichert
</commit_message>
<xml_diff>
--- a/Twitch-Spediteur/ExterneDateien/Entfernungen.xlsx
+++ b/Twitch-Spediteur/ExterneDateien/Entfernungen.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Games\Twitch-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Twitch-Spediteur\Twitch-Spediteur\ExterneDateien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8B21A42-E05B-4B47-8B73-05CDED6A7ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECCA28D-D639-4FA9-B7DF-A9FD911F580C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DE674BBA-4DCB-499B-AC3F-14CAC4005E9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -119,7 +120,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,13 +128,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,13 +158,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Akzent1" xfId="1" builtinId="29"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -467,7 +483,7 @@
   <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="W33" sqref="W33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,128 +598,1967 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="1"/>
+      <c r="C2">
+        <v>170</v>
+      </c>
+      <c r="D2">
+        <v>150</v>
+      </c>
+      <c r="E2">
+        <v>405</v>
+      </c>
+      <c r="F2">
+        <v>448</v>
+      </c>
+      <c r="G2">
+        <v>482</v>
+      </c>
+      <c r="H2">
+        <v>462</v>
+      </c>
+      <c r="I2">
+        <v>465</v>
+      </c>
+      <c r="J2">
+        <v>392</v>
+      </c>
+      <c r="K2">
+        <v>441</v>
+      </c>
+      <c r="L2">
+        <v>655</v>
+      </c>
+      <c r="M2">
+        <v>631</v>
+      </c>
+      <c r="N2">
+        <v>218</v>
+      </c>
+      <c r="O2">
+        <v>285</v>
+      </c>
+      <c r="P2">
+        <v>750</v>
+      </c>
+      <c r="Q2">
+        <v>109</v>
+      </c>
+      <c r="R2">
+        <v>60</v>
+      </c>
+      <c r="S2">
+        <v>348</v>
+      </c>
+      <c r="T2">
+        <v>227</v>
+      </c>
+      <c r="U2">
+        <v>228</v>
+      </c>
+      <c r="V2">
+        <v>310</v>
+      </c>
+      <c r="W2">
+        <v>339</v>
+      </c>
+      <c r="X2">
+        <v>374</v>
+      </c>
+      <c r="Y2">
+        <v>10</v>
+      </c>
+      <c r="Z2">
+        <v>479</v>
+      </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>170</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3">
+        <v>80</v>
+      </c>
+      <c r="E3">
+        <v>573</v>
+      </c>
+      <c r="F3">
+        <v>615</v>
+      </c>
+      <c r="G3">
+        <v>650</v>
+      </c>
+      <c r="H3">
+        <v>630</v>
+      </c>
+      <c r="I3">
+        <v>632</v>
+      </c>
+      <c r="J3">
+        <v>560</v>
+      </c>
+      <c r="K3">
+        <v>590</v>
+      </c>
+      <c r="L3">
+        <v>802</v>
+      </c>
+      <c r="M3">
+        <v>778</v>
+      </c>
+      <c r="N3">
+        <v>232</v>
+      </c>
+      <c r="O3">
+        <v>430</v>
+      </c>
+      <c r="P3">
+        <v>897</v>
+      </c>
+      <c r="Q3">
+        <v>277</v>
+      </c>
+      <c r="R3">
+        <v>204</v>
+      </c>
+      <c r="S3">
+        <v>516</v>
+      </c>
+      <c r="T3">
+        <v>394</v>
+      </c>
+      <c r="U3">
+        <v>396</v>
+      </c>
+      <c r="V3">
+        <v>478</v>
+      </c>
+      <c r="W3">
+        <v>500</v>
+      </c>
+      <c r="X3">
+        <v>440</v>
+      </c>
+      <c r="Y3">
+        <v>174</v>
+      </c>
+      <c r="Z3">
+        <v>646</v>
+      </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>150</v>
+      </c>
+      <c r="C4">
+        <v>80</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4">
+        <v>522</v>
+      </c>
+      <c r="F4">
+        <v>564</v>
+      </c>
+      <c r="G4">
+        <v>597</v>
+      </c>
+      <c r="H4">
+        <v>578</v>
+      </c>
+      <c r="I4">
+        <v>581</v>
+      </c>
+      <c r="J4">
+        <v>502</v>
+      </c>
+      <c r="K4">
+        <v>569</v>
+      </c>
+      <c r="L4">
+        <v>805</v>
+      </c>
+      <c r="M4">
+        <v>740</v>
+      </c>
+      <c r="N4">
+        <v>164</v>
+      </c>
+      <c r="O4">
+        <v>415</v>
+      </c>
+      <c r="P4">
+        <v>862</v>
+      </c>
+      <c r="Q4">
+        <v>246</v>
+      </c>
+      <c r="R4">
+        <v>123</v>
+      </c>
+      <c r="S4">
+        <v>485</v>
+      </c>
+      <c r="T4">
+        <v>360</v>
+      </c>
+      <c r="U4">
+        <v>372</v>
+      </c>
+      <c r="V4">
+        <v>446</v>
+      </c>
+      <c r="W4">
+        <v>432</v>
+      </c>
+      <c r="X4">
+        <v>372</v>
+      </c>
+      <c r="Y4">
+        <v>153</v>
+      </c>
+      <c r="Z4">
+        <v>595</v>
+      </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>405</v>
+      </c>
+      <c r="C5">
+        <v>573</v>
+      </c>
+      <c r="D5">
+        <v>522</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5">
+        <v>45</v>
+      </c>
+      <c r="G5">
+        <v>87</v>
+      </c>
+      <c r="H5">
+        <v>102</v>
+      </c>
+      <c r="I5">
+        <v>70</v>
+      </c>
+      <c r="J5">
+        <v>29</v>
+      </c>
+      <c r="K5">
+        <v>573</v>
+      </c>
+      <c r="L5">
+        <v>432</v>
+      </c>
+      <c r="M5">
+        <v>315</v>
+      </c>
+      <c r="N5">
+        <v>368</v>
+      </c>
+      <c r="O5">
+        <v>497</v>
+      </c>
+      <c r="P5">
+        <v>509</v>
+      </c>
+      <c r="Q5">
+        <v>301</v>
+      </c>
+      <c r="R5">
+        <v>384</v>
+      </c>
+      <c r="S5">
+        <v>92</v>
+      </c>
+      <c r="T5">
+        <v>190</v>
+      </c>
+      <c r="U5">
+        <v>367</v>
+      </c>
+      <c r="V5">
+        <v>242</v>
+      </c>
+      <c r="W5">
+        <v>109</v>
+      </c>
+      <c r="X5">
+        <v>259</v>
+      </c>
+      <c r="Y5">
+        <v>401</v>
+      </c>
+      <c r="Z5">
+        <v>87</v>
+      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>448</v>
+      </c>
+      <c r="C6">
+        <v>615</v>
+      </c>
+      <c r="D6">
+        <v>564</v>
+      </c>
+      <c r="E6">
+        <v>45</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6">
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <v>70</v>
+      </c>
+      <c r="I6">
+        <v>35</v>
+      </c>
+      <c r="J6">
+        <v>76</v>
+      </c>
+      <c r="K6">
+        <v>561</v>
+      </c>
+      <c r="L6">
+        <v>402</v>
+      </c>
+      <c r="M6">
+        <v>292</v>
+      </c>
+      <c r="N6">
+        <v>409</v>
+      </c>
+      <c r="O6">
+        <v>485</v>
+      </c>
+      <c r="P6">
+        <v>487</v>
+      </c>
+      <c r="Q6">
+        <v>342</v>
+      </c>
+      <c r="R6">
+        <v>425</v>
+      </c>
+      <c r="S6">
+        <v>132</v>
+      </c>
+      <c r="T6">
+        <v>231</v>
+      </c>
+      <c r="U6">
+        <v>382</v>
+      </c>
+      <c r="V6">
+        <v>230</v>
+      </c>
+      <c r="W6">
+        <v>156</v>
+      </c>
+      <c r="X6">
+        <v>306</v>
+      </c>
+      <c r="Y6">
+        <v>441</v>
+      </c>
+      <c r="Z6">
+        <v>85</v>
+      </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>482</v>
+      </c>
+      <c r="C7">
+        <v>650</v>
+      </c>
+      <c r="D7">
+        <v>597</v>
+      </c>
+      <c r="E7">
+        <v>87</v>
+      </c>
+      <c r="F7">
+        <v>50</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7">
+        <v>23</v>
+      </c>
+      <c r="I7">
+        <v>17</v>
+      </c>
+      <c r="J7">
+        <v>114</v>
+      </c>
+      <c r="K7">
+        <v>517</v>
+      </c>
+      <c r="L7">
+        <v>376</v>
+      </c>
+      <c r="M7">
+        <v>259</v>
+      </c>
+      <c r="N7">
+        <v>443</v>
+      </c>
+      <c r="O7">
+        <v>436</v>
+      </c>
+      <c r="P7">
+        <v>454</v>
+      </c>
+      <c r="Q7">
+        <v>375</v>
+      </c>
+      <c r="R7">
+        <v>457</v>
+      </c>
+      <c r="S7">
+        <v>123</v>
+      </c>
+      <c r="T7">
+        <v>265</v>
+      </c>
+      <c r="U7">
+        <v>333</v>
+      </c>
+      <c r="V7">
+        <v>181</v>
+      </c>
+      <c r="W7">
+        <v>180</v>
+      </c>
+      <c r="X7">
+        <v>339</v>
+      </c>
+      <c r="Y7">
+        <v>475</v>
+      </c>
+      <c r="Z7">
+        <v>138</v>
+      </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>462</v>
+      </c>
+      <c r="C8">
+        <v>630</v>
+      </c>
+      <c r="D8">
+        <v>578</v>
+      </c>
+      <c r="E8">
+        <v>102</v>
+      </c>
+      <c r="F8">
+        <v>70</v>
+      </c>
+      <c r="G8">
+        <v>23</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8">
+        <v>37</v>
+      </c>
+      <c r="J8">
+        <v>121</v>
+      </c>
+      <c r="K8">
+        <v>493</v>
+      </c>
+      <c r="L8">
+        <v>352</v>
+      </c>
+      <c r="M8">
+        <v>235</v>
+      </c>
+      <c r="N8">
+        <v>450</v>
+      </c>
+      <c r="O8">
+        <v>417</v>
+      </c>
+      <c r="P8">
+        <v>429</v>
+      </c>
+      <c r="Q8">
+        <v>360</v>
+      </c>
+      <c r="R8">
+        <v>437</v>
+      </c>
+      <c r="S8">
+        <v>106</v>
+      </c>
+      <c r="T8">
+        <v>225</v>
+      </c>
+      <c r="U8">
+        <v>314</v>
+      </c>
+      <c r="V8">
+        <v>161</v>
+      </c>
+      <c r="W8">
+        <v>188</v>
+      </c>
+      <c r="X8">
+        <v>351</v>
+      </c>
+      <c r="Y8">
+        <v>456</v>
+      </c>
+      <c r="Z8">
+        <v>158</v>
+      </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>465</v>
+      </c>
+      <c r="C9">
+        <v>632</v>
+      </c>
+      <c r="D9">
+        <v>581</v>
+      </c>
+      <c r="E9">
+        <v>70</v>
+      </c>
+      <c r="F9">
+        <v>35</v>
+      </c>
+      <c r="G9">
+        <v>17</v>
+      </c>
+      <c r="H9">
+        <v>37</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9">
+        <v>99</v>
+      </c>
+      <c r="K9">
+        <v>528</v>
+      </c>
+      <c r="L9">
+        <v>362</v>
+      </c>
+      <c r="M9">
+        <v>251</v>
+      </c>
+      <c r="N9">
+        <v>428</v>
+      </c>
+      <c r="O9">
+        <v>451</v>
+      </c>
+      <c r="P9">
+        <v>446</v>
+      </c>
+      <c r="Q9">
+        <v>361</v>
+      </c>
+      <c r="R9">
+        <v>444</v>
+      </c>
+      <c r="S9">
+        <v>151</v>
+      </c>
+      <c r="T9">
+        <v>250</v>
+      </c>
+      <c r="U9">
+        <v>349</v>
+      </c>
+      <c r="V9">
+        <v>196</v>
+      </c>
+      <c r="W9">
+        <v>165</v>
+      </c>
+      <c r="X9">
+        <v>329</v>
+      </c>
+      <c r="Y9">
+        <v>460</v>
+      </c>
+      <c r="Z9">
+        <v>123</v>
+      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10">
+        <v>392</v>
+      </c>
+      <c r="C10">
+        <v>560</v>
+      </c>
+      <c r="D10">
+        <v>502</v>
+      </c>
+      <c r="E10">
+        <v>29</v>
+      </c>
+      <c r="F10">
+        <v>76</v>
+      </c>
+      <c r="G10">
+        <v>114</v>
+      </c>
+      <c r="H10">
+        <v>121</v>
+      </c>
+      <c r="I10">
+        <v>99</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10">
+        <v>601</v>
+      </c>
+      <c r="L10">
+        <v>455</v>
+      </c>
+      <c r="M10">
+        <v>338</v>
+      </c>
+      <c r="N10">
+        <v>349</v>
+      </c>
+      <c r="O10">
+        <v>498</v>
+      </c>
+      <c r="P10">
+        <v>533</v>
+      </c>
+      <c r="Q10">
+        <v>284</v>
+      </c>
+      <c r="R10">
+        <v>367</v>
+      </c>
+      <c r="S10">
+        <v>115</v>
+      </c>
+      <c r="T10">
+        <v>173</v>
+      </c>
+      <c r="U10">
+        <v>364</v>
+      </c>
+      <c r="V10">
+        <v>265</v>
+      </c>
+      <c r="W10">
+        <v>62</v>
+      </c>
+      <c r="X10">
+        <v>239</v>
+      </c>
+      <c r="Y10">
+        <v>383</v>
+      </c>
+      <c r="Z10">
+        <v>97</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11">
+        <v>441</v>
+      </c>
+      <c r="C11">
+        <v>590</v>
+      </c>
+      <c r="D11">
+        <v>569</v>
+      </c>
+      <c r="E11">
+        <v>573</v>
+      </c>
+      <c r="F11">
+        <v>561</v>
+      </c>
+      <c r="G11">
+        <v>517</v>
+      </c>
+      <c r="H11">
+        <v>493</v>
+      </c>
+      <c r="I11">
+        <v>528</v>
+      </c>
+      <c r="J11">
+        <v>601</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11">
+        <v>290</v>
+      </c>
+      <c r="M11">
+        <v>399</v>
+      </c>
+      <c r="N11">
+        <v>636</v>
+      </c>
+      <c r="O11">
+        <v>195</v>
+      </c>
+      <c r="P11">
+        <v>356</v>
+      </c>
+      <c r="Q11">
+        <v>487</v>
+      </c>
+      <c r="R11">
+        <v>486</v>
+      </c>
+      <c r="S11">
+        <v>579</v>
+      </c>
+      <c r="T11">
+        <v>550</v>
+      </c>
+      <c r="U11">
+        <v>305</v>
+      </c>
+      <c r="V11">
+        <v>385</v>
+      </c>
+      <c r="W11">
+        <v>606</v>
+      </c>
+      <c r="X11">
+        <v>737</v>
+      </c>
+      <c r="Y11">
+        <v>460</v>
+      </c>
+      <c r="Z11">
+        <v>644</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12">
+        <v>655</v>
+      </c>
+      <c r="C12">
+        <v>802</v>
+      </c>
+      <c r="D12">
+        <v>805</v>
+      </c>
+      <c r="E12">
+        <v>432</v>
+      </c>
+      <c r="F12">
+        <v>402</v>
+      </c>
+      <c r="G12">
+        <v>376</v>
+      </c>
+      <c r="H12">
+        <v>352</v>
+      </c>
+      <c r="I12">
+        <v>362</v>
+      </c>
+      <c r="J12">
+        <v>455</v>
+      </c>
+      <c r="K12">
+        <v>290</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12">
+        <v>126</v>
+      </c>
+      <c r="N12">
+        <v>663</v>
+      </c>
+      <c r="O12">
+        <v>396</v>
+      </c>
+      <c r="P12">
+        <v>97</v>
+      </c>
+      <c r="Q12">
+        <v>517</v>
+      </c>
+      <c r="R12">
+        <v>593</v>
+      </c>
+      <c r="S12">
+        <v>444</v>
+      </c>
+      <c r="T12">
+        <v>501</v>
+      </c>
+      <c r="U12">
+        <v>396</v>
+      </c>
+      <c r="V12">
+        <v>318</v>
+      </c>
+      <c r="W12">
+        <v>525</v>
+      </c>
+      <c r="X12">
+        <v>689</v>
+      </c>
+      <c r="Y12">
+        <v>661</v>
+      </c>
+      <c r="Z12">
+        <v>498</v>
+      </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13">
+        <v>631</v>
+      </c>
+      <c r="C13">
+        <v>778</v>
+      </c>
+      <c r="D13">
+        <v>740</v>
+      </c>
+      <c r="E13">
+        <v>315</v>
+      </c>
+      <c r="F13">
+        <v>292</v>
+      </c>
+      <c r="G13">
+        <v>259</v>
+      </c>
+      <c r="H13">
+        <v>235</v>
+      </c>
+      <c r="I13">
+        <v>251</v>
+      </c>
+      <c r="J13">
+        <v>338</v>
+      </c>
+      <c r="K13">
+        <v>399</v>
+      </c>
+      <c r="L13">
+        <v>126</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13">
+        <v>671</v>
+      </c>
+      <c r="O13">
+        <v>373</v>
+      </c>
+      <c r="P13">
+        <v>212</v>
+      </c>
+      <c r="Q13">
+        <v>504</v>
+      </c>
+      <c r="R13">
+        <v>580</v>
+      </c>
+      <c r="S13">
+        <v>327</v>
+      </c>
+      <c r="T13">
+        <v>446</v>
+      </c>
+      <c r="U13">
+        <v>373</v>
+      </c>
+      <c r="V13">
+        <v>305</v>
+      </c>
+      <c r="W13">
+        <v>408</v>
+      </c>
+      <c r="X13">
+        <v>572</v>
+      </c>
+      <c r="Y13">
+        <v>639</v>
+      </c>
+      <c r="Z13">
+        <v>380</v>
+      </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="B14">
+        <v>218</v>
+      </c>
+      <c r="C14">
+        <v>232</v>
+      </c>
+      <c r="D14">
+        <v>164</v>
+      </c>
+      <c r="E14">
+        <v>368</v>
+      </c>
+      <c r="F14">
+        <v>409</v>
+      </c>
+      <c r="G14">
+        <v>443</v>
+      </c>
+      <c r="H14">
+        <v>450</v>
+      </c>
+      <c r="I14">
+        <v>428</v>
+      </c>
+      <c r="J14">
+        <v>349</v>
+      </c>
+      <c r="K14">
+        <v>636</v>
+      </c>
+      <c r="L14">
+        <v>663</v>
+      </c>
+      <c r="M14">
+        <v>671</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14">
+        <v>473</v>
+      </c>
+      <c r="P14">
+        <v>811</v>
+      </c>
+      <c r="Q14">
+        <v>147</v>
+      </c>
+      <c r="R14">
+        <v>152</v>
+      </c>
+      <c r="S14">
+        <v>328</v>
+      </c>
+      <c r="T14">
+        <v>203</v>
+      </c>
+      <c r="U14">
+        <v>339</v>
+      </c>
+      <c r="V14">
+        <v>356</v>
+      </c>
+      <c r="W14">
+        <v>276</v>
+      </c>
+      <c r="X14">
+        <v>218</v>
+      </c>
+      <c r="Y14">
+        <v>215</v>
+      </c>
+      <c r="Z14">
+        <v>439</v>
+      </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
+      <c r="B15">
+        <v>285</v>
+      </c>
+      <c r="C15">
+        <v>430</v>
+      </c>
+      <c r="D15">
+        <v>415</v>
+      </c>
+      <c r="E15">
+        <v>497</v>
+      </c>
+      <c r="F15">
+        <v>485</v>
+      </c>
+      <c r="G15">
+        <v>436</v>
+      </c>
+      <c r="H15">
+        <v>417</v>
+      </c>
+      <c r="I15">
+        <v>451</v>
+      </c>
+      <c r="J15">
+        <v>498</v>
+      </c>
+      <c r="K15">
+        <v>195</v>
+      </c>
+      <c r="L15">
+        <v>396</v>
+      </c>
+      <c r="M15">
+        <v>373</v>
+      </c>
+      <c r="N15">
+        <v>473</v>
+      </c>
+      <c r="O15" s="1"/>
+      <c r="P15">
+        <v>492</v>
+      </c>
+      <c r="Q15">
+        <v>337</v>
+      </c>
+      <c r="R15">
+        <v>326</v>
+      </c>
+      <c r="S15">
+        <v>419</v>
+      </c>
+      <c r="T15">
+        <v>391</v>
+      </c>
+      <c r="U15">
+        <v>162</v>
+      </c>
+      <c r="V15">
+        <v>254</v>
+      </c>
+      <c r="W15">
+        <v>446</v>
+      </c>
+      <c r="X15">
+        <v>566</v>
+      </c>
+      <c r="Y15">
+        <v>300</v>
+      </c>
+      <c r="Z15">
+        <v>562</v>
+      </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
+      <c r="B16">
+        <v>750</v>
+      </c>
+      <c r="C16">
+        <v>897</v>
+      </c>
+      <c r="D16">
+        <v>862</v>
+      </c>
+      <c r="E16">
+        <v>509</v>
+      </c>
+      <c r="F16">
+        <v>487</v>
+      </c>
+      <c r="G16">
+        <v>454</v>
+      </c>
+      <c r="H16">
+        <v>429</v>
+      </c>
+      <c r="I16">
+        <v>446</v>
+      </c>
+      <c r="J16">
+        <v>533</v>
+      </c>
+      <c r="K16">
+        <v>356</v>
+      </c>
+      <c r="L16">
+        <v>97</v>
+      </c>
+      <c r="M16">
+        <v>212</v>
+      </c>
+      <c r="N16">
+        <v>811</v>
+      </c>
+      <c r="O16">
+        <v>492</v>
+      </c>
+      <c r="P16" s="1"/>
+      <c r="Q16">
+        <v>612</v>
+      </c>
+      <c r="R16">
+        <v>689</v>
+      </c>
+      <c r="S16">
+        <v>521</v>
+      </c>
+      <c r="T16">
+        <v>596</v>
+      </c>
+      <c r="U16">
+        <v>492</v>
+      </c>
+      <c r="V16">
+        <v>414</v>
+      </c>
+      <c r="W16">
+        <v>603</v>
+      </c>
+      <c r="X16">
+        <v>767</v>
+      </c>
+      <c r="Y16">
+        <v>757</v>
+      </c>
+      <c r="Z16">
+        <v>575</v>
+      </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
+      <c r="B17">
+        <v>109</v>
+      </c>
+      <c r="C17">
+        <v>277</v>
+      </c>
+      <c r="D17">
+        <v>246</v>
+      </c>
+      <c r="E17">
+        <v>301</v>
+      </c>
+      <c r="F17">
+        <v>342</v>
+      </c>
+      <c r="G17">
+        <v>375</v>
+      </c>
+      <c r="H17">
+        <v>360</v>
+      </c>
+      <c r="I17">
+        <v>361</v>
+      </c>
+      <c r="J17">
+        <v>284</v>
+      </c>
+      <c r="K17">
+        <v>487</v>
+      </c>
+      <c r="L17">
+        <v>517</v>
+      </c>
+      <c r="M17">
+        <v>504</v>
+      </c>
+      <c r="N17">
+        <v>147</v>
+      </c>
+      <c r="O17">
+        <v>337</v>
+      </c>
+      <c r="P17">
+        <v>612</v>
+      </c>
+      <c r="Q17" s="1"/>
+      <c r="R17">
+        <v>86</v>
+      </c>
+      <c r="S17">
+        <v>242</v>
+      </c>
+      <c r="T17">
+        <v>121</v>
+      </c>
+      <c r="U17">
+        <v>193</v>
+      </c>
+      <c r="V17">
+        <v>210</v>
+      </c>
+      <c r="W17">
+        <v>233</v>
+      </c>
+      <c r="X17">
+        <v>292</v>
+      </c>
+      <c r="Y17">
+        <v>104</v>
+      </c>
+      <c r="Z17">
+        <v>373</v>
+      </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
+      <c r="B18">
+        <v>60</v>
+      </c>
+      <c r="C18">
+        <v>204</v>
+      </c>
+      <c r="D18">
+        <v>123</v>
+      </c>
+      <c r="E18">
+        <v>384</v>
+      </c>
+      <c r="F18">
+        <v>425</v>
+      </c>
+      <c r="G18">
+        <v>457</v>
+      </c>
+      <c r="H18">
+        <v>437</v>
+      </c>
+      <c r="I18">
+        <v>444</v>
+      </c>
+      <c r="J18">
+        <v>367</v>
+      </c>
+      <c r="K18">
+        <v>486</v>
+      </c>
+      <c r="L18">
+        <v>593</v>
+      </c>
+      <c r="M18">
+        <v>580</v>
+      </c>
+      <c r="N18">
+        <v>152</v>
+      </c>
+      <c r="O18">
+        <v>326</v>
+      </c>
+      <c r="P18">
+        <v>689</v>
+      </c>
+      <c r="Q18">
+        <v>86</v>
+      </c>
+      <c r="R18" s="1"/>
+      <c r="S18">
+        <v>327</v>
+      </c>
+      <c r="T18">
+        <v>205</v>
+      </c>
+      <c r="U18">
+        <v>289</v>
+      </c>
+      <c r="V18">
+        <v>286</v>
+      </c>
+      <c r="W18">
+        <v>318</v>
+      </c>
+      <c r="X18">
+        <v>316</v>
+      </c>
+      <c r="Y18">
+        <v>70</v>
+      </c>
+      <c r="Z18">
+        <v>457</v>
+      </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
+      <c r="B19">
+        <v>348</v>
+      </c>
+      <c r="C19">
+        <v>516</v>
+      </c>
+      <c r="D19">
+        <v>485</v>
+      </c>
+      <c r="E19">
+        <v>92</v>
+      </c>
+      <c r="F19">
+        <v>132</v>
+      </c>
+      <c r="G19">
+        <v>123</v>
+      </c>
+      <c r="H19">
+        <v>106</v>
+      </c>
+      <c r="I19">
+        <v>151</v>
+      </c>
+      <c r="J19">
+        <v>115</v>
+      </c>
+      <c r="K19">
+        <v>579</v>
+      </c>
+      <c r="L19">
+        <v>444</v>
+      </c>
+      <c r="M19">
+        <v>327</v>
+      </c>
+      <c r="N19">
+        <v>328</v>
+      </c>
+      <c r="O19">
+        <v>419</v>
+      </c>
+      <c r="P19">
+        <v>521</v>
+      </c>
+      <c r="Q19">
+        <v>242</v>
+      </c>
+      <c r="R19">
+        <v>327</v>
+      </c>
+      <c r="S19" s="1"/>
+      <c r="T19">
+        <v>131</v>
+      </c>
+      <c r="U19">
+        <v>287</v>
+      </c>
+      <c r="V19">
+        <v>170</v>
+      </c>
+      <c r="W19">
+        <v>103</v>
+      </c>
+      <c r="X19">
+        <v>294</v>
+      </c>
+      <c r="Y19">
+        <v>342</v>
+      </c>
+      <c r="Z19">
+        <v>172</v>
+      </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
+      <c r="B20">
+        <v>227</v>
+      </c>
+      <c r="C20">
+        <v>394</v>
+      </c>
+      <c r="D20">
+        <v>360</v>
+      </c>
+      <c r="E20">
+        <v>190</v>
+      </c>
+      <c r="F20">
+        <v>231</v>
+      </c>
+      <c r="G20">
+        <v>265</v>
+      </c>
+      <c r="H20">
+        <v>225</v>
+      </c>
+      <c r="I20">
+        <v>250</v>
+      </c>
+      <c r="J20">
+        <v>173</v>
+      </c>
+      <c r="K20">
+        <v>550</v>
+      </c>
+      <c r="L20">
+        <v>501</v>
+      </c>
+      <c r="M20">
+        <v>446</v>
+      </c>
+      <c r="N20">
+        <v>203</v>
+      </c>
+      <c r="O20">
+        <v>391</v>
+      </c>
+      <c r="P20">
+        <v>596</v>
+      </c>
+      <c r="Q20">
+        <v>121</v>
+      </c>
+      <c r="R20">
+        <v>205</v>
+      </c>
+      <c r="S20">
+        <v>131</v>
+      </c>
+      <c r="T20" s="1"/>
+      <c r="U20">
+        <v>262</v>
+      </c>
+      <c r="V20">
+        <v>198</v>
+      </c>
+      <c r="W20">
+        <v>123</v>
+      </c>
+      <c r="X20">
+        <v>182</v>
+      </c>
+      <c r="Y20">
+        <v>219</v>
+      </c>
+      <c r="Z20">
+        <v>262</v>
+      </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
+      <c r="B21">
+        <v>228</v>
+      </c>
+      <c r="C21">
+        <v>396</v>
+      </c>
+      <c r="D21">
+        <v>372</v>
+      </c>
+      <c r="E21">
+        <v>367</v>
+      </c>
+      <c r="F21">
+        <v>382</v>
+      </c>
+      <c r="G21">
+        <v>333</v>
+      </c>
+      <c r="H21">
+        <v>314</v>
+      </c>
+      <c r="I21">
+        <v>349</v>
+      </c>
+      <c r="J21">
+        <v>364</v>
+      </c>
+      <c r="K21">
+        <v>305</v>
+      </c>
+      <c r="L21">
+        <v>396</v>
+      </c>
+      <c r="M21">
+        <v>373</v>
+      </c>
+      <c r="N21">
+        <v>339</v>
+      </c>
+      <c r="O21">
+        <v>162</v>
+      </c>
+      <c r="P21">
+        <v>492</v>
+      </c>
+      <c r="Q21">
+        <v>193</v>
+      </c>
+      <c r="R21">
+        <v>289</v>
+      </c>
+      <c r="S21">
+        <v>287</v>
+      </c>
+      <c r="T21">
+        <v>262</v>
+      </c>
+      <c r="U21" s="1"/>
+      <c r="V21">
+        <v>194</v>
+      </c>
+      <c r="W21">
+        <v>312</v>
+      </c>
+      <c r="X21">
+        <v>433</v>
+      </c>
+      <c r="Y21">
+        <v>225</v>
+      </c>
+      <c r="Z21">
+        <v>445</v>
+      </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
+      <c r="B22">
+        <v>310</v>
+      </c>
+      <c r="C22">
+        <v>478</v>
+      </c>
+      <c r="D22">
+        <v>446</v>
+      </c>
+      <c r="E22">
+        <v>242</v>
+      </c>
+      <c r="F22">
+        <v>230</v>
+      </c>
+      <c r="G22">
+        <v>181</v>
+      </c>
+      <c r="H22">
+        <v>161</v>
+      </c>
+      <c r="I22">
+        <v>196</v>
+      </c>
+      <c r="J22">
+        <v>265</v>
+      </c>
+      <c r="K22">
+        <v>385</v>
+      </c>
+      <c r="L22">
+        <v>318</v>
+      </c>
+      <c r="M22">
+        <v>305</v>
+      </c>
+      <c r="N22">
+        <v>356</v>
+      </c>
+      <c r="O22">
+        <v>254</v>
+      </c>
+      <c r="P22">
+        <v>414</v>
+      </c>
+      <c r="Q22">
+        <v>210</v>
+      </c>
+      <c r="R22">
+        <v>286</v>
+      </c>
+      <c r="S22">
+        <v>170</v>
+      </c>
+      <c r="T22">
+        <v>198</v>
+      </c>
+      <c r="U22">
+        <v>194</v>
+      </c>
+      <c r="V22" s="1"/>
+      <c r="W22">
+        <v>248</v>
+      </c>
+      <c r="X22">
+        <v>369</v>
+      </c>
+      <c r="Y22">
+        <v>304</v>
+      </c>
+      <c r="Z22">
+        <v>311</v>
+      </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
+      <c r="B23">
+        <v>339</v>
+      </c>
+      <c r="C23">
+        <v>500</v>
+      </c>
+      <c r="D23">
+        <v>432</v>
+      </c>
+      <c r="E23">
+        <v>109</v>
+      </c>
+      <c r="F23">
+        <v>156</v>
+      </c>
+      <c r="G23">
+        <v>180</v>
+      </c>
+      <c r="H23">
+        <v>188</v>
+      </c>
+      <c r="I23">
+        <v>165</v>
+      </c>
+      <c r="J23">
+        <v>62</v>
+      </c>
+      <c r="K23">
+        <v>606</v>
+      </c>
+      <c r="L23">
+        <v>525</v>
+      </c>
+      <c r="M23">
+        <v>408</v>
+      </c>
+      <c r="N23">
+        <v>276</v>
+      </c>
+      <c r="O23">
+        <v>446</v>
+      </c>
+      <c r="P23">
+        <v>603</v>
+      </c>
+      <c r="Q23">
+        <v>233</v>
+      </c>
+      <c r="R23">
+        <v>318</v>
+      </c>
+      <c r="S23">
+        <v>103</v>
+      </c>
+      <c r="T23">
+        <v>123</v>
+      </c>
+      <c r="U23">
+        <v>312</v>
+      </c>
+      <c r="V23">
+        <v>248</v>
+      </c>
+      <c r="W23" s="1"/>
+      <c r="X23">
+        <v>200</v>
+      </c>
+      <c r="Y23">
+        <v>335</v>
+      </c>
+      <c r="Z23">
+        <v>174</v>
+      </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
+      <c r="B24">
+        <v>374</v>
+      </c>
+      <c r="C24">
+        <v>440</v>
+      </c>
+      <c r="D24">
+        <v>372</v>
+      </c>
+      <c r="E24">
+        <v>259</v>
+      </c>
+      <c r="F24">
+        <v>306</v>
+      </c>
+      <c r="G24">
+        <v>339</v>
+      </c>
+      <c r="H24">
+        <v>351</v>
+      </c>
+      <c r="I24">
+        <v>329</v>
+      </c>
+      <c r="J24">
+        <v>239</v>
+      </c>
+      <c r="K24">
+        <v>737</v>
+      </c>
+      <c r="L24">
+        <v>689</v>
+      </c>
+      <c r="M24">
+        <v>572</v>
+      </c>
+      <c r="N24">
+        <v>218</v>
+      </c>
+      <c r="O24">
+        <v>566</v>
+      </c>
+      <c r="P24">
+        <v>767</v>
+      </c>
+      <c r="Q24">
+        <v>292</v>
+      </c>
+      <c r="R24">
+        <v>316</v>
+      </c>
+      <c r="S24">
+        <v>294</v>
+      </c>
+      <c r="T24">
+        <v>182</v>
+      </c>
+      <c r="U24">
+        <v>433</v>
+      </c>
+      <c r="V24">
+        <v>369</v>
+      </c>
+      <c r="W24">
+        <v>200</v>
+      </c>
+      <c r="X24" s="1"/>
+      <c r="Y24">
+        <v>373</v>
+      </c>
+      <c r="Z24">
+        <v>262</v>
+      </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>174</v>
+      </c>
+      <c r="D25">
+        <v>153</v>
+      </c>
+      <c r="E25">
+        <v>401</v>
+      </c>
+      <c r="F25">
+        <v>441</v>
+      </c>
+      <c r="G25">
+        <v>475</v>
+      </c>
+      <c r="H25">
+        <v>456</v>
+      </c>
+      <c r="I25">
+        <v>460</v>
+      </c>
+      <c r="J25">
+        <v>383</v>
+      </c>
+      <c r="K25">
+        <v>460</v>
+      </c>
+      <c r="L25">
+        <v>661</v>
+      </c>
+      <c r="M25">
+        <v>639</v>
+      </c>
+      <c r="N25">
+        <v>215</v>
+      </c>
+      <c r="O25">
+        <v>300</v>
+      </c>
+      <c r="P25">
+        <v>757</v>
+      </c>
+      <c r="Q25">
+        <v>104</v>
+      </c>
+      <c r="R25">
+        <v>70</v>
+      </c>
+      <c r="S25">
+        <v>342</v>
+      </c>
+      <c r="T25">
+        <v>219</v>
+      </c>
+      <c r="U25">
+        <v>225</v>
+      </c>
+      <c r="V25">
+        <v>304</v>
+      </c>
+      <c r="W25">
+        <v>335</v>
+      </c>
+      <c r="X25">
+        <v>373</v>
+      </c>
+      <c r="Y25" s="1"/>
+      <c r="Z25">
+        <v>473</v>
+      </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
+      <c r="B26">
+        <v>479</v>
+      </c>
+      <c r="C26">
+        <v>646</v>
+      </c>
+      <c r="D26">
+        <v>595</v>
+      </c>
+      <c r="E26">
+        <v>87</v>
+      </c>
+      <c r="F26">
+        <v>85</v>
+      </c>
+      <c r="G26">
+        <v>138</v>
+      </c>
+      <c r="H26">
+        <v>158</v>
+      </c>
+      <c r="I26">
+        <v>123</v>
+      </c>
+      <c r="J26">
+        <v>97</v>
+      </c>
+      <c r="K26">
+        <v>644</v>
+      </c>
+      <c r="L26">
+        <v>498</v>
+      </c>
+      <c r="M26">
+        <v>380</v>
+      </c>
+      <c r="N26">
+        <v>439</v>
+      </c>
+      <c r="O26">
+        <v>562</v>
+      </c>
+      <c r="P26">
+        <v>575</v>
+      </c>
+      <c r="Q26">
+        <v>373</v>
+      </c>
+      <c r="R26">
+        <v>457</v>
+      </c>
+      <c r="S26">
+        <v>172</v>
+      </c>
+      <c r="T26">
+        <v>262</v>
+      </c>
+      <c r="U26">
+        <v>445</v>
+      </c>
+      <c r="V26">
+        <v>311</v>
+      </c>
+      <c r="W26">
+        <v>174</v>
+      </c>
+      <c r="X26">
+        <v>262</v>
+      </c>
+      <c r="Y26">
+        <v>473</v>
+      </c>
+      <c r="Z26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD21458-3326-45C9-9745-072B65289752}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T1" sqref="A1:T1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>